<commit_message>
Se realiza la actualización del dashboard 20230306
</commit_message>
<xml_diff>
--- a/Informes/Sabana_Notas_1s/Sabana_Notas_1s.xlsx
+++ b/Informes/Sabana_Notas_1s/Sabana_Notas_1s.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
   <si>
     <t>Radicado</t>
   </si>
@@ -598,6 +598,57 @@
   </si>
   <si>
     <t>3185302133</t>
+  </si>
+  <si>
+    <t>2:33 p.m.</t>
+  </si>
+  <si>
+    <t>Maria Claudia Acosta Guerra</t>
+  </si>
+  <si>
+    <t>97112621575</t>
+  </si>
+  <si>
+    <t>acostaguerra@gmail.com</t>
+  </si>
+  <si>
+    <t>TÉCNICO LABORAL POR COMPETENCIAS EN OPERACIÓN DE PROGRAMAS INFORMÁTICOS Y BASES DE DATOS</t>
+  </si>
+  <si>
+    <t>1019135840</t>
+  </si>
+  <si>
+    <t>21/02/2023</t>
+  </si>
+  <si>
+    <t>3114866604</t>
+  </si>
+  <si>
+    <t>10:21 a.m.</t>
+  </si>
+  <si>
+    <t>Diego Mora Pereira</t>
+  </si>
+  <si>
+    <t>1030701629</t>
+  </si>
+  <si>
+    <t>diegomorapereira1012@gmail.com</t>
+  </si>
+  <si>
+    <t>TÉCNICO LABORAL POR COMPETENCIAS EN SEGURIDAD OCUPACIONAL</t>
+  </si>
+  <si>
+    <t>TÉCNICO LABORAL POR COMPETENCIAS EN AUXILIAR DE SEGURIDAD EN EL TRABAJO</t>
+  </si>
+  <si>
+    <t>24/02/2023</t>
+  </si>
+  <si>
+    <t>3102896885</t>
+  </si>
+  <si>
+    <t>ya termine la carrera</t>
   </si>
 </sst>
 </file>
@@ -659,8 +710,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SolicitudInstitucionalReporteViewModel_1" displayName="SolicitudInstitucionalReporteViewModel_1" ref="A1:AA27">
-  <autoFilter ref="A1:AA27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SolicitudInstitucionalReporteViewModel_1" displayName="SolicitudInstitucionalReporteViewModel_1" ref="A1:AA29">
+  <autoFilter ref="A1:AA29"/>
   <tableColumns count="27">
     <tableColumn id="1" name="Radicado"/>
     <tableColumn id="2" name="Tiempo en Transito"/>
@@ -696,7 +747,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA28"/>
+  <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -711,7 +762,7 @@
     <col min="7" max="7" width="37.1964530944824" customWidth="1"/>
     <col min="8" max="8" width="30.9322242736816" customWidth="1"/>
     <col min="9" max="9" width="35.617862701416" customWidth="1"/>
-    <col min="10" max="10" width="81.90234375" customWidth="1"/>
+    <col min="10" max="10" width="96.5536651611328" customWidth="1"/>
     <col min="11" max="11" width="17.5937786102295" customWidth="1"/>
     <col min="12" max="12" width="30.3961372375488" customWidth="1"/>
     <col min="13" max="13" width="21.0742473602295" customWidth="1"/>
@@ -722,7 +773,7 @@
     <col min="18" max="18" width="31.8092708587646" customWidth="1"/>
     <col min="19" max="19" width="33.0962867736816" customWidth="1"/>
     <col min="20" max="20" width="22.4512920379639" customWidth="1"/>
-    <col min="21" max="21" width="81.90234375" customWidth="1"/>
+    <col min="21" max="21" width="96.5536651611328" customWidth="1"/>
     <col min="22" max="22" width="21.1946887969971" customWidth="1"/>
     <col min="23" max="23" width="19.3616352081299" customWidth="1"/>
     <col min="24" max="24" width="52.5365676879883" customWidth="1"/>
@@ -819,7 +870,7 @@
         <v>59554</v>
       </c>
       <c r="B2" s="5">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C2" s="6">
         <v>44930.5085256944</v>
@@ -902,7 +953,7 @@
         <v>59554</v>
       </c>
       <c r="B3" s="5">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C3" s="6">
         <v>44930.5085256944</v>
@@ -985,7 +1036,7 @@
         <v>59613</v>
       </c>
       <c r="B4" s="5">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C4" s="6">
         <v>44931.4907380787</v>
@@ -1068,7 +1119,7 @@
         <v>59613</v>
       </c>
       <c r="B5" s="5">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6">
         <v>44931.4907380787</v>
@@ -1151,7 +1202,7 @@
         <v>59866</v>
       </c>
       <c r="B6" s="5">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C6" s="6">
         <v>44937.564937581</v>
@@ -1224,7 +1275,7 @@
         <v>59921</v>
       </c>
       <c r="B7" s="5">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6">
         <v>44938.3978695949</v>
@@ -1307,7 +1358,7 @@
         <v>59921</v>
       </c>
       <c r="B8" s="5">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6">
         <v>44938.3978695949</v>
@@ -1390,7 +1441,7 @@
         <v>59933</v>
       </c>
       <c r="B9" s="5">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6">
         <v>44938.4796079514</v>
@@ -1463,7 +1514,7 @@
         <v>60015</v>
       </c>
       <c r="B10" s="5">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C10" s="6">
         <v>44939.3781462963</v>
@@ -1546,7 +1597,7 @@
         <v>60015</v>
       </c>
       <c r="B11" s="5">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C11" s="6">
         <v>44939.3781462963</v>
@@ -1629,7 +1680,7 @@
         <v>60331</v>
       </c>
       <c r="B12" s="5">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C12" s="6">
         <v>44944.4020761574</v>
@@ -1712,7 +1763,7 @@
         <v>60331</v>
       </c>
       <c r="B13" s="5">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C13" s="6">
         <v>44944.4020761574</v>
@@ -1795,7 +1846,7 @@
         <v>60358</v>
       </c>
       <c r="B14" s="5">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C14" s="6">
         <v>44944.5479141204</v>
@@ -1878,7 +1929,7 @@
         <v>60358</v>
       </c>
       <c r="B15" s="5">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C15" s="6">
         <v>44944.5479141204</v>
@@ -1961,7 +2012,7 @@
         <v>60894</v>
       </c>
       <c r="B16" s="5">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C16" s="6">
         <v>44950.6821927083</v>
@@ -2034,7 +2085,7 @@
         <v>61397</v>
       </c>
       <c r="B17" s="5">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C17" s="6">
         <v>44956.6890259607</v>
@@ -2107,7 +2158,7 @@
         <v>61402</v>
       </c>
       <c r="B18" s="5">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C18" s="6">
         <v>44956.6961732639</v>
@@ -2180,7 +2231,7 @@
         <v>61404</v>
       </c>
       <c r="B19" s="5">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C19" s="6">
         <v>44956.7041137732</v>
@@ -2253,7 +2304,7 @@
         <v>61574</v>
       </c>
       <c r="B20" s="5">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C20" s="6">
         <v>44957.851291169</v>
@@ -2336,7 +2387,7 @@
         <v>61620</v>
       </c>
       <c r="B21" s="5">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C21" s="6">
         <v>44958.4445203357</v>
@@ -2419,7 +2470,7 @@
         <v>61760</v>
       </c>
       <c r="B22" s="5">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C22" s="6">
         <v>44959.6836011227</v>
@@ -2492,7 +2543,7 @@
         <v>61916</v>
       </c>
       <c r="B23" s="5">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C23" s="6">
         <v>44960.8203810532</v>
@@ -2565,7 +2616,7 @@
         <v>62173</v>
       </c>
       <c r="B24" s="5">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C24" s="6">
         <v>44963.4935478356</v>
@@ -2638,7 +2689,7 @@
         <v>62680</v>
       </c>
       <c r="B25" s="5">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C25" s="6">
         <v>44965.3014347222</v>
@@ -2711,7 +2762,7 @@
         <v>63108</v>
       </c>
       <c r="B26" s="5">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C26" s="6">
         <v>44966.6582956829</v>
@@ -2794,7 +2845,7 @@
         <v>63108</v>
       </c>
       <c r="B27" s="5">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C27" s="6">
         <v>44966.6582956829</v>
@@ -2873,32 +2924,178 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
-      <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
-      <c r="Z28" s="3"/>
-      <c r="AA28" s="3"/>
+      <c r="A28" s="5">
+        <v>65029</v>
+      </c>
+      <c r="B28" s="5">
+        <v>13</v>
+      </c>
+      <c r="C28" s="6">
+        <v>44978.6064027778</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R28" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="S28" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="T28" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="U28" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="V28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="W28" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="X28" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y28" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z28" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA28" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5">
+        <v>65321</v>
+      </c>
+      <c r="B29" s="5">
+        <v>10</v>
+      </c>
+      <c r="C29" s="6">
+        <v>44981.4316254282</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="T29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y29" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z29" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA29" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
     </row>
   </sheetData>
   <headerFooter/>

</xml_diff>